<commit_message>
Update string resources with differentiation algorithms
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/PR translation.xlsx
+++ b/SignalAnalysis/localization/PR translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD9866A-F9FB-4CCD-B43E-24288AFE38C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A5335-ACC4-4216-A245-8F189622F291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F4122FDA-4629-4765-8032-FD9A5F537F26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="76">
   <si>
     <t>Key</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>strDifferentiationAlgorithms</t>
+  </si>
+  <si>
+    <t>In plot derivative. Please take into account that "seconds" is abbreviated so that it fits in the ordinate axis.</t>
   </si>
 </sst>
 </file>
@@ -365,10 +368,10 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,24 +387,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P29" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P29" totalsRowShown="0" dataDxfId="15">
   <autoFilter ref="B2:P29" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{065EC89B-5B24-4DE2-8CDC-71C71F8644F1}" name="Key" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{ACC4F180-1DF1-4E86-A34A-9E1E5BCA4825}" name="Comment" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{5AF3FBAE-5FB4-42DD-A7CF-16181E305FC0}" name="English" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{2DF9BC46-12E9-4A95-84CD-1B44A71D026C}" name=".ar" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{ADAD8BFB-2ABE-441D-8BB8-784262A9C605}" name=".bn-BD" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{ACD337BE-2060-4846-A3EC-9620B0468CF1}" name=".da-DK" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{281E3D2D-3165-4A98-BC40-CB71BBAE1FBD}" name=".nl-BE" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{C7B5C606-BAD1-4326-8D3B-0C7C5A520763}" name=".de-DE" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{0B2C0086-FAA6-4F3C-AFB6-9977B68A3BD5}" name=".hi-IN" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{144B1478-1EA9-4B3A-A1E8-B8C82582874D}" name=".it-IT" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{221EB64D-BF23-4561-8A54-4683408656C3}" name=".lt-LT" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{CF182762-6C95-435E-A2A4-933ACCE6E0CF}" name=".nb-NO" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{77DC50D9-63AE-47D3-8D8D-73E1EA53D699}" name=".pt-BR" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{442AD067-4C0E-44F1-A612-018D96E77EEB}" name=".ru-RU" dataDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{178B2CEE-AD39-4CCC-9137-81E5E55CF179}" name=".tr-TR" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{065EC89B-5B24-4DE2-8CDC-71C71F8644F1}" name="Key" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{ACC4F180-1DF1-4E86-A34A-9E1E5BCA4825}" name="Comment" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5AF3FBAE-5FB4-42DD-A7CF-16181E305FC0}" name="English" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{2DF9BC46-12E9-4A95-84CD-1B44A71D026C}" name=".ar" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{ADAD8BFB-2ABE-441D-8BB8-784262A9C605}" name=".bn-BD" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{ACD337BE-2060-4846-A3EC-9620B0468CF1}" name=".da-DK" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{281E3D2D-3165-4A98-BC40-CB71BBAE1FBD}" name=".nl-BE" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{C7B5C606-BAD1-4326-8D3B-0C7C5A520763}" name=".de-DE" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{0B2C0086-FAA6-4F3C-AFB6-9977B68A3BD5}" name=".hi-IN" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{144B1478-1EA9-4B3A-A1E8-B8C82582874D}" name=".it-IT" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{221EB64D-BF23-4561-8A54-4683408656C3}" name=".lt-LT" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{CF182762-6C95-435E-A2A4-933ACCE6E0CF}" name=".nb-NO" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{77DC50D9-63AE-47D3-8D8D-73E1EA53D699}" name=".pt-BR" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{442AD067-4C0E-44F1-A612-018D96E77EEB}" name=".ru-RU" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{178B2CEE-AD39-4CCC-9137-81E5E55CF179}" name=".tr-TR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1825,7 +1828,7 @@
         <v>66</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Add additional string to be translated
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/PR translation.xlsx
+++ b/SignalAnalysis/localization/PR translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A5335-ACC4-4216-A245-8F189622F291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5643E823-E2E0-4CD2-85DE-A9B922A2D991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F4122FDA-4629-4765-8032-FD9A5F537F26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="79">
   <si>
     <t>Key</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>In plot derivative. Please take into account that "seconds" is abbreviated so that it fits in the ordinate axis.</t>
+  </si>
+  <si>
+    <t>strFileHeader29</t>
+  </si>
+  <si>
+    <t>Differentiation algorithm</t>
+  </si>
+  <si>
+    <t>Field description in exported file</t>
   </si>
 </sst>
 </file>
@@ -387,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P29" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="B2:P29" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P30" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="B2:P30" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{065EC89B-5B24-4DE2-8CDC-71C71F8644F1}" name="Key" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{ACC4F180-1DF1-4E86-A34A-9E1E5BCA4825}" name="Comment" dataDxfId="13"/>
@@ -707,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9850087B-4788-4433-A763-D052FACB1285}">
-  <dimension ref="B2:P29"/>
+  <dimension ref="B2:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1939,6 +1948,29 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add Excel file for Russian translation
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/PR translation.xlsx
+++ b/SignalAnalysis/localization/PR translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\source\repos\SignalAnalysis\SignalAnalysis\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A53BA8-C436-436D-92F3-98D22B6DB1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4A8F0-2276-4E29-A088-11592B4F119E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F4122FDA-4629-4765-8032-FD9A5F537F26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="89">
   <si>
     <t>Key</t>
   </si>
@@ -161,33 +161,6 @@
   </si>
   <si>
     <t>Amplitude</t>
-  </si>
-  <si>
-    <t>strRadCentralFive</t>
-  </si>
-  <si>
-    <t>In "settings" form, mathematical name</t>
-  </si>
-  <si>
-    <t>Central five-point difference</t>
-  </si>
-  <si>
-    <t>strRadCentralThree</t>
-  </si>
-  <si>
-    <t>Central three-point difference</t>
-  </si>
-  <si>
-    <t>strRadForwardOne</t>
-  </si>
-  <si>
-    <t>Forward one-point difference</t>
-  </si>
-  <si>
-    <t>strRadBackwardOne</t>
-  </si>
-  <si>
-    <t>Backward one-point difference</t>
   </si>
   <si>
     <t>strGrpAlgorithms</t>
@@ -453,8 +426,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P39" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="B2:P39" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}" name="Tabla1" displayName="Tabla1" ref="B2:P35" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="B2:P35" xr:uid="{8D5FF1DE-9302-4D24-B533-72ECE4B8891D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P35">
+    <sortCondition ref="B2:B35"/>
+  </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{065EC89B-5B24-4DE2-8CDC-71C71F8644F1}" name="Key" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{ACC4F180-1DF1-4E86-A34A-9E1E5BCA4825}" name="Comment" dataDxfId="13"/>
@@ -773,7 +749,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9850087B-4788-4433-A763-D052FACB1285}">
-  <dimension ref="B2:P39"/>
+  <dimension ref="B2:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -793,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -834,60 +810,36 @@
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -928,60 +880,36 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
@@ -1022,295 +950,151 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" ht="120" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
@@ -1349,109 +1133,61 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>2</v>
@@ -1492,13 +1228,13 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2</v>
@@ -1539,13 +1275,13 @@
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>2</v>
@@ -1586,13 +1322,13 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>2</v>
@@ -1633,13 +1369,13 @@
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>2</v>
@@ -1680,13 +1416,13 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>2</v>
@@ -1727,13 +1463,13 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>2</v>
@@ -1774,13 +1510,13 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>2</v>
@@ -1821,13 +1557,13 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>2</v>
@@ -1868,82 +1604,154 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>2</v>
@@ -1982,15 +1790,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:16" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>73</v>
+        <v>42</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2007,13 +1815,13 @@
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2030,59 +1838,107 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -2099,36 +1955,60 @@
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-    </row>
-    <row r="35" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>95</v>
+        <v>52</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2143,98 +2023,6 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>